<commit_message>
Check data and modification statistical treatment
</commit_message>
<xml_diff>
--- a/stream3_visualization/Well-being/output/completeness.xlsx
+++ b/stream3_visualization/Well-being/output/completeness.xlsx
@@ -13,9 +13,9 @@
     <sheet name="ES-SILC-1" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="ES-SILC-2" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="HE-SILC-1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="HE-SILC-2" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="HQ-SILC-1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="RU-SILC-1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="HQ-SILC-1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="RU-SILC-1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="HE-SILC-2" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="AH-SILC-4" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="RT-LFS-1" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="RT-LFS-2" sheetId="12" state="visible" r:id="rId12"/>
@@ -54241,10 +54241,10 @@
         <v>10</v>
       </c>
       <c r="T4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -54674,7 +54674,7 @@
         <v>10</v>
       </c>
       <c r="H11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>10</v>
@@ -55103,19 +55103,19 @@
         <v>10</v>
       </c>
       <c r="Q17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="T17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -55158,19 +55158,19 @@
         <v>10</v>
       </c>
       <c r="M18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R18" t="n">
         <v>10</v>
@@ -55380,10 +55380,10 @@
         <v>10</v>
       </c>
       <c r="T21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -55447,7 +55447,7 @@
         <v>10</v>
       </c>
       <c r="T22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U22" t="n">
         <v>10</v>
@@ -55514,10 +55514,10 @@
         <v>10</v>
       </c>
       <c r="T23" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U23" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -56117,10 +56117,10 @@
         <v>10</v>
       </c>
       <c r="T32" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U32" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -56471,10 +56471,10 @@
         <v>10</v>
       </c>
       <c r="T4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -56904,7 +56904,7 @@
         <v>10</v>
       </c>
       <c r="H11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>10</v>
@@ -57333,19 +57333,19 @@
         <v>10</v>
       </c>
       <c r="Q17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="T17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -57610,10 +57610,10 @@
         <v>10</v>
       </c>
       <c r="T21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -57677,7 +57677,7 @@
         <v>10</v>
       </c>
       <c r="T22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U22" t="n">
         <v>10</v>
@@ -57744,10 +57744,10 @@
         <v>10</v>
       </c>
       <c r="T23" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U23" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -58347,10 +58347,10 @@
         <v>10</v>
       </c>
       <c r="T32" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U32" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -58513,16 +58513,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>10</v>
@@ -58580,16 +58580,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>10</v>
@@ -58647,22 +58647,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>10</v>
       </c>
       <c r="G4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>10</v>
@@ -58701,10 +58701,10 @@
         <v>10</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -58714,16 +58714,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>10</v>
@@ -58781,16 +58781,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>10</v>
@@ -58848,16 +58848,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>10</v>
@@ -58915,16 +58915,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>10</v>
@@ -58982,25 +58982,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
         <v>10</v>
@@ -59049,16 +59049,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>10</v>
@@ -59116,25 +59116,25 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>10</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I11" t="n">
         <v>10</v>
@@ -59183,16 +59183,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>10</v>
@@ -59250,25 +59250,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>10</v>
       </c>
       <c r="G13" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>10</v>
@@ -59317,16 +59317,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
         <v>10</v>
@@ -59384,25 +59384,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
         <v>10</v>
@@ -59454,13 +59454,13 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>10</v>
@@ -59521,13 +59521,13 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>10</v>
@@ -59563,19 +59563,19 @@
         <v>10</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T17" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U17" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -59588,22 +59588,22 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
         <v>10</v>
@@ -59655,19 +59655,19 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>10</v>
@@ -59722,13 +59722,13 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>10</v>
@@ -59789,10 +59789,10 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -59840,10 +59840,10 @@
         <v>10</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U21" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -59856,13 +59856,13 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>10</v>
@@ -59907,7 +59907,7 @@
         <v>10</v>
       </c>
       <c r="T22" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U22" t="n">
         <v>10</v>
@@ -59923,13 +59923,13 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
         <v>10</v>
@@ -59974,10 +59974,10 @@
         <v>10</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U23" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -59990,13 +59990,13 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
         <v>10</v>
@@ -60057,13 +60057,13 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
         <v>10</v>
@@ -60124,22 +60124,22 @@
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
         <v>10</v>
@@ -60197,7 +60197,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
         <v>10</v>
@@ -60264,7 +60264,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
         <v>10</v>
@@ -60331,10 +60331,10 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
         <v>10</v>
@@ -60398,7 +60398,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
         <v>10</v>
@@ -60577,10 +60577,10 @@
         <v>10</v>
       </c>
       <c r="T32" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U32" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33">

</xml_diff>